<commit_message>
moved file structure around
</commit_message>
<xml_diff>
--- a/BestBall/DK5.xlsx
+++ b/BestBall/DK5.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\splee\Documents\BestBallGit\Fantasy-Football-and-Betting\BestBall\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ECEA44C-B593-4AFC-8877-6D28E4425A40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9408F013-6A31-4853-AC89-B209EF0521BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12120" yWindow="45" windowWidth="12210" windowHeight="14025" xr2:uid="{3C7CEAA8-2282-44F1-AA06-C995D9B81E2D}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11790" windowHeight="14280" xr2:uid="{3C7CEAA8-2282-44F1-AA06-C995D9B81E2D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1211" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1311" uniqueCount="200">
   <si>
     <t>Team</t>
   </si>
@@ -614,6 +614,27 @@
   </si>
   <si>
     <t>Hassan Haskins</t>
+  </si>
+  <si>
+    <t>Jamar Chase</t>
+  </si>
+  <si>
+    <t>Rashod Bateman</t>
+  </si>
+  <si>
+    <t>Chase Claypool</t>
+  </si>
+  <si>
+    <t>Pat Freiermuth</t>
+  </si>
+  <si>
+    <t>Isaiah Spiller</t>
+  </si>
+  <si>
+    <t>Jamison Crowder</t>
+  </si>
+  <si>
+    <t>James White</t>
   </si>
 </sst>
 </file>
@@ -966,10 +987,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D088BB7-28FF-48AE-BA8A-D751F5557836}">
-  <dimension ref="A1:L241"/>
+  <dimension ref="A1:L261"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A209" workbookViewId="0">
-      <selection activeCell="B242" sqref="B242"/>
+    <sheetView tabSelected="1" topLeftCell="B220" workbookViewId="0">
+      <selection activeCell="F261" sqref="F261"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1086,7 +1107,7 @@
         <v>44694</v>
       </c>
       <c r="J3">
-        <f t="shared" ref="J3:J22" si="1">SUM(H$2:H$21)</f>
+        <f t="shared" ref="J3:J21" si="1">SUM(H$2:H$21)</f>
         <v>94.3</v>
       </c>
       <c r="K3" t="s">
@@ -1886,7 +1907,7 @@
         <v>44694</v>
       </c>
       <c r="J23">
-        <f t="shared" ref="J23:J42" si="2">SUM(H$22:H$41)</f>
+        <f t="shared" ref="J23:J41" si="2">SUM(H$22:H$41)</f>
         <v>112.79999999999998</v>
       </c>
       <c r="K23" t="s">
@@ -2686,7 +2707,7 @@
         <v>44694</v>
       </c>
       <c r="J43">
-        <f t="shared" ref="J43:J62" si="3">SUM(H$42:H$61)</f>
+        <f t="shared" ref="J43:J61" si="3">SUM(H$42:H$61)</f>
         <v>71.099999999999994</v>
       </c>
       <c r="K43" t="s">
@@ -3483,7 +3504,7 @@
         <v>44694</v>
       </c>
       <c r="J63">
-        <f t="shared" ref="J63:J82" si="4">SUM(H$62:H$81)</f>
+        <f t="shared" ref="J63:J81" si="4">SUM(H$62:H$81)</f>
         <v>54.300000000000004</v>
       </c>
       <c r="K63" t="s">
@@ -4283,7 +4304,7 @@
         <v>44694</v>
       </c>
       <c r="J83">
-        <f t="shared" ref="J83:J102" si="6">SUM(H$82:H$101)</f>
+        <f t="shared" ref="J83:J101" si="6">SUM(H$82:H$101)</f>
         <v>221.5</v>
       </c>
       <c r="K83" t="s">
@@ -5083,7 +5104,7 @@
         <v>44694</v>
       </c>
       <c r="J103">
-        <f t="shared" ref="J103:J122" si="7">SUM(H$102:H$121)</f>
+        <f t="shared" ref="J103:J121" si="7">SUM(H$102:H$121)</f>
         <v>46.299999999999976</v>
       </c>
       <c r="K103" t="s">
@@ -5883,7 +5904,7 @@
         <v>44695</v>
       </c>
       <c r="J123">
-        <f t="shared" ref="J123:J142" si="8">SUM(H$122:H$141)</f>
+        <f t="shared" ref="J123:J141" si="8">SUM(H$122:H$141)</f>
         <v>74.900000000000034</v>
       </c>
       <c r="K123" t="s">
@@ -6683,7 +6704,7 @@
         <v>44695</v>
       </c>
       <c r="J143">
-        <f t="shared" ref="J143:J162" si="10">SUM(H$142:H$161)</f>
+        <f t="shared" ref="J143:J161" si="10">SUM(H$142:H$161)</f>
         <v>84.299999999999983</v>
       </c>
       <c r="K143" t="s">
@@ -7483,7 +7504,7 @@
         <v>44695</v>
       </c>
       <c r="J163">
-        <f t="shared" ref="J163:J182" si="11">SUM(H$162:H$181)</f>
+        <f t="shared" ref="J163:J181" si="11">SUM(H$162:H$181)</f>
         <v>32.899999999999991</v>
       </c>
       <c r="K163" t="s">
@@ -8283,7 +8304,7 @@
         <v>44695</v>
       </c>
       <c r="J183">
-        <f t="shared" ref="J183:J202" si="12">SUM(H$182:H$201)</f>
+        <f t="shared" ref="J183:J201" si="12">SUM(H$182:H$201)</f>
         <v>43.9</v>
       </c>
       <c r="K183" t="s">
@@ -8756,7 +8777,7 @@
         <v>158.5</v>
       </c>
       <c r="H195">
-        <f t="shared" ref="H195:H241" si="13">F195-G195</f>
+        <f t="shared" ref="H195:H240" si="13">F195-G195</f>
         <v>9.5</v>
       </c>
       <c r="I195" s="1">
@@ -9083,7 +9104,7 @@
         <v>44696</v>
       </c>
       <c r="J203">
-        <f t="shared" ref="J203:J222" si="14">SUM(H$202:H$221)</f>
+        <f t="shared" ref="J203:J221" si="14">SUM(H$202:H$221)</f>
         <v>67.5</v>
       </c>
       <c r="K203" t="s">
@@ -9883,7 +9904,7 @@
         <v>44696</v>
       </c>
       <c r="J223">
-        <f t="shared" ref="J223:J241" si="15">SUM(H$222:H$241)</f>
+        <f t="shared" ref="J223:J242" si="15">SUM(H$222:H$241)</f>
         <v>96.200000000000017</v>
       </c>
       <c r="K223" t="s">
@@ -10611,6 +10632,806 @@
       </c>
       <c r="L241" t="s">
         <v>126</v>
+      </c>
+    </row>
+    <row r="242" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A242">
+        <v>13</v>
+      </c>
+      <c r="B242" t="s">
+        <v>26</v>
+      </c>
+      <c r="C242" t="s">
+        <v>193</v>
+      </c>
+      <c r="D242" t="s">
+        <v>104</v>
+      </c>
+      <c r="E242">
+        <v>1</v>
+      </c>
+      <c r="F242">
+        <v>6</v>
+      </c>
+      <c r="G242">
+        <v>4.8</v>
+      </c>
+      <c r="H242">
+        <f>F242-G242</f>
+        <v>1.2000000000000002</v>
+      </c>
+      <c r="I242" s="1">
+        <v>44697</v>
+      </c>
+      <c r="J242">
+        <f>SUM(H$242:H$261)</f>
+        <v>60.6</v>
+      </c>
+      <c r="K242" t="s">
+        <v>118</v>
+      </c>
+      <c r="L242" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="243" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A243">
+        <v>13</v>
+      </c>
+      <c r="B243" t="s">
+        <v>15</v>
+      </c>
+      <c r="C243" t="s">
+        <v>16</v>
+      </c>
+      <c r="D243" t="s">
+        <v>17</v>
+      </c>
+      <c r="E243">
+        <v>2</v>
+      </c>
+      <c r="F243">
+        <v>19</v>
+      </c>
+      <c r="G243">
+        <v>18.5</v>
+      </c>
+      <c r="H243">
+        <f t="shared" ref="H243:H261" si="16">F243-G243</f>
+        <v>0.5</v>
+      </c>
+      <c r="I243" s="1">
+        <v>44697</v>
+      </c>
+      <c r="J243">
+        <f t="shared" ref="J243:J261" si="17">SUM(H$242:H$261)</f>
+        <v>60.6</v>
+      </c>
+      <c r="K243" t="s">
+        <v>118</v>
+      </c>
+      <c r="L243" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="244" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A244">
+        <v>13</v>
+      </c>
+      <c r="B244" t="s">
+        <v>12</v>
+      </c>
+      <c r="C244" t="s">
+        <v>72</v>
+      </c>
+      <c r="D244" t="s">
+        <v>30</v>
+      </c>
+      <c r="E244">
+        <v>3</v>
+      </c>
+      <c r="F244">
+        <v>30</v>
+      </c>
+      <c r="G244">
+        <v>26.2</v>
+      </c>
+      <c r="H244">
+        <f t="shared" si="16"/>
+        <v>3.8000000000000007</v>
+      </c>
+      <c r="I244" s="1">
+        <v>44697</v>
+      </c>
+      <c r="J244">
+        <f t="shared" si="17"/>
+        <v>60.6</v>
+      </c>
+      <c r="K244" t="s">
+        <v>118</v>
+      </c>
+      <c r="L244" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="245" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A245">
+        <v>13</v>
+      </c>
+      <c r="B245" t="s">
+        <v>28</v>
+      </c>
+      <c r="C245" t="s">
+        <v>129</v>
+      </c>
+      <c r="D245" t="s">
+        <v>17</v>
+      </c>
+      <c r="E245">
+        <v>4</v>
+      </c>
+      <c r="F245">
+        <v>43</v>
+      </c>
+      <c r="G245">
+        <v>44.1</v>
+      </c>
+      <c r="H245">
+        <f t="shared" si="16"/>
+        <v>-1.1000000000000014</v>
+      </c>
+      <c r="I245" s="1">
+        <v>44697</v>
+      </c>
+      <c r="J245">
+        <f t="shared" si="17"/>
+        <v>60.6</v>
+      </c>
+      <c r="K245" t="s">
+        <v>118</v>
+      </c>
+      <c r="L245" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="246" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A246">
+        <v>13</v>
+      </c>
+      <c r="B246" t="s">
+        <v>26</v>
+      </c>
+      <c r="C246" t="s">
+        <v>62</v>
+      </c>
+      <c r="D246" t="s">
+        <v>61</v>
+      </c>
+      <c r="E246">
+        <v>5</v>
+      </c>
+      <c r="F246">
+        <v>54</v>
+      </c>
+      <c r="G246">
+        <v>48.3</v>
+      </c>
+      <c r="H246">
+        <f t="shared" si="16"/>
+        <v>5.7000000000000028</v>
+      </c>
+      <c r="I246" s="1">
+        <v>44697</v>
+      </c>
+      <c r="J246">
+        <f t="shared" si="17"/>
+        <v>60.6</v>
+      </c>
+      <c r="K246" t="s">
+        <v>118</v>
+      </c>
+      <c r="L246" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="247" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A247">
+        <v>13</v>
+      </c>
+      <c r="B247" t="s">
+        <v>26</v>
+      </c>
+      <c r="C247" t="s">
+        <v>194</v>
+      </c>
+      <c r="D247" t="s">
+        <v>17</v>
+      </c>
+      <c r="E247">
+        <v>6</v>
+      </c>
+      <c r="F247">
+        <v>67</v>
+      </c>
+      <c r="G247">
+        <v>68.599999999999994</v>
+      </c>
+      <c r="H247">
+        <f t="shared" si="16"/>
+        <v>-1.5999999999999943</v>
+      </c>
+      <c r="I247" s="1">
+        <v>44697</v>
+      </c>
+      <c r="J247">
+        <f t="shared" si="17"/>
+        <v>60.6</v>
+      </c>
+      <c r="K247" t="s">
+        <v>118</v>
+      </c>
+      <c r="L247" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="248" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A248">
+        <v>13</v>
+      </c>
+      <c r="B248" t="s">
+        <v>26</v>
+      </c>
+      <c r="C248" t="s">
+        <v>64</v>
+      </c>
+      <c r="D248" t="s">
+        <v>65</v>
+      </c>
+      <c r="E248">
+        <v>7</v>
+      </c>
+      <c r="F248">
+        <v>78</v>
+      </c>
+      <c r="G248">
+        <v>79.099999999999994</v>
+      </c>
+      <c r="H248">
+        <f t="shared" si="16"/>
+        <v>-1.0999999999999943</v>
+      </c>
+      <c r="I248" s="1">
+        <v>44697</v>
+      </c>
+      <c r="J248">
+        <f t="shared" si="17"/>
+        <v>60.6</v>
+      </c>
+      <c r="K248" t="s">
+        <v>118</v>
+      </c>
+      <c r="L248" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="249" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A249">
+        <v>13</v>
+      </c>
+      <c r="B249" t="s">
+        <v>26</v>
+      </c>
+      <c r="C249" t="s">
+        <v>168</v>
+      </c>
+      <c r="D249" t="s">
+        <v>70</v>
+      </c>
+      <c r="E249">
+        <v>8</v>
+      </c>
+      <c r="F249">
+        <v>91</v>
+      </c>
+      <c r="G249">
+        <v>89.3</v>
+      </c>
+      <c r="H249">
+        <f t="shared" si="16"/>
+        <v>1.7000000000000028</v>
+      </c>
+      <c r="I249" s="1">
+        <v>44697</v>
+      </c>
+      <c r="J249">
+        <f t="shared" si="17"/>
+        <v>60.6</v>
+      </c>
+      <c r="K249" t="s">
+        <v>118</v>
+      </c>
+      <c r="L249" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="250" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A250">
+        <v>13</v>
+      </c>
+      <c r="B250" t="s">
+        <v>28</v>
+      </c>
+      <c r="C250" t="s">
+        <v>80</v>
+      </c>
+      <c r="D250" t="s">
+        <v>70</v>
+      </c>
+      <c r="E250">
+        <v>9</v>
+      </c>
+      <c r="F250">
+        <v>102</v>
+      </c>
+      <c r="G250">
+        <v>98.1</v>
+      </c>
+      <c r="H250">
+        <f t="shared" si="16"/>
+        <v>3.9000000000000057</v>
+      </c>
+      <c r="I250" s="1">
+        <v>44697</v>
+      </c>
+      <c r="J250">
+        <f t="shared" si="17"/>
+        <v>60.6</v>
+      </c>
+      <c r="K250" t="s">
+        <v>118</v>
+      </c>
+      <c r="L250" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="251" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A251">
+        <v>13</v>
+      </c>
+      <c r="B251" t="s">
+        <v>26</v>
+      </c>
+      <c r="C251" t="s">
+        <v>195</v>
+      </c>
+      <c r="D251" t="s">
+        <v>52</v>
+      </c>
+      <c r="E251">
+        <v>10</v>
+      </c>
+      <c r="F251">
+        <v>115</v>
+      </c>
+      <c r="G251">
+        <v>111</v>
+      </c>
+      <c r="H251">
+        <f t="shared" si="16"/>
+        <v>4</v>
+      </c>
+      <c r="I251" s="1">
+        <v>44697</v>
+      </c>
+      <c r="J251">
+        <f t="shared" si="17"/>
+        <v>60.6</v>
+      </c>
+      <c r="K251" t="s">
+        <v>118</v>
+      </c>
+      <c r="L251" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="252" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A252">
+        <v>13</v>
+      </c>
+      <c r="B252" t="s">
+        <v>15</v>
+      </c>
+      <c r="C252" t="s">
+        <v>196</v>
+      </c>
+      <c r="D252" t="s">
+        <v>52</v>
+      </c>
+      <c r="E252">
+        <v>11</v>
+      </c>
+      <c r="F252">
+        <v>126</v>
+      </c>
+      <c r="G252">
+        <v>118.2</v>
+      </c>
+      <c r="H252">
+        <f t="shared" si="16"/>
+        <v>7.7999999999999972</v>
+      </c>
+      <c r="I252" s="1">
+        <v>44697</v>
+      </c>
+      <c r="J252">
+        <f t="shared" si="17"/>
+        <v>60.6</v>
+      </c>
+      <c r="K252" t="s">
+        <v>118</v>
+      </c>
+      <c r="L252" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="253" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A253">
+        <v>13</v>
+      </c>
+      <c r="B253" t="s">
+        <v>12</v>
+      </c>
+      <c r="C253" t="s">
+        <v>197</v>
+      </c>
+      <c r="D253" t="s">
+        <v>141</v>
+      </c>
+      <c r="E253">
+        <v>12</v>
+      </c>
+      <c r="F253">
+        <v>139</v>
+      </c>
+      <c r="G253">
+        <v>134.30000000000001</v>
+      </c>
+      <c r="H253">
+        <f t="shared" si="16"/>
+        <v>4.6999999999999886</v>
+      </c>
+      <c r="I253" s="1">
+        <v>44697</v>
+      </c>
+      <c r="J253">
+        <f t="shared" si="17"/>
+        <v>60.6</v>
+      </c>
+      <c r="K253" t="s">
+        <v>118</v>
+      </c>
+      <c r="L253" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="254" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A254">
+        <v>13</v>
+      </c>
+      <c r="B254" t="s">
+        <v>26</v>
+      </c>
+      <c r="C254" t="s">
+        <v>198</v>
+      </c>
+      <c r="D254" t="s">
+        <v>138</v>
+      </c>
+      <c r="E254">
+        <v>13</v>
+      </c>
+      <c r="F254">
+        <v>150</v>
+      </c>
+      <c r="G254">
+        <v>148.1</v>
+      </c>
+      <c r="H254">
+        <f t="shared" si="16"/>
+        <v>1.9000000000000057</v>
+      </c>
+      <c r="I254" s="1">
+        <v>44697</v>
+      </c>
+      <c r="J254">
+        <f t="shared" si="17"/>
+        <v>60.6</v>
+      </c>
+      <c r="K254" t="s">
+        <v>118</v>
+      </c>
+      <c r="L254" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="255" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A255">
+        <v>13</v>
+      </c>
+      <c r="B255" t="s">
+        <v>12</v>
+      </c>
+      <c r="C255" t="s">
+        <v>95</v>
+      </c>
+      <c r="D255" t="s">
+        <v>23</v>
+      </c>
+      <c r="E255">
+        <v>14</v>
+      </c>
+      <c r="F255">
+        <v>163</v>
+      </c>
+      <c r="G255">
+        <v>151.9</v>
+      </c>
+      <c r="H255">
+        <f t="shared" si="16"/>
+        <v>11.099999999999994</v>
+      </c>
+      <c r="I255" s="1">
+        <v>44697</v>
+      </c>
+      <c r="J255">
+        <f t="shared" si="17"/>
+        <v>60.6</v>
+      </c>
+      <c r="K255" t="s">
+        <v>118</v>
+      </c>
+      <c r="L255" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="256" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A256">
+        <v>13</v>
+      </c>
+      <c r="B256" t="s">
+        <v>12</v>
+      </c>
+      <c r="C256" t="s">
+        <v>93</v>
+      </c>
+      <c r="D256" t="s">
+        <v>94</v>
+      </c>
+      <c r="E256">
+        <v>15</v>
+      </c>
+      <c r="F256">
+        <v>174</v>
+      </c>
+      <c r="G256">
+        <v>172</v>
+      </c>
+      <c r="H256">
+        <f t="shared" si="16"/>
+        <v>2</v>
+      </c>
+      <c r="I256" s="1">
+        <v>44697</v>
+      </c>
+      <c r="J256">
+        <f t="shared" si="17"/>
+        <v>60.6</v>
+      </c>
+      <c r="K256" t="s">
+        <v>118</v>
+      </c>
+      <c r="L256" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="257" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A257">
+        <v>13</v>
+      </c>
+      <c r="B257" t="s">
+        <v>12</v>
+      </c>
+      <c r="C257" t="s">
+        <v>186</v>
+      </c>
+      <c r="D257" t="s">
+        <v>70</v>
+      </c>
+      <c r="E257">
+        <v>16</v>
+      </c>
+      <c r="F257">
+        <v>187</v>
+      </c>
+      <c r="G257">
+        <v>177</v>
+      </c>
+      <c r="H257">
+        <f t="shared" si="16"/>
+        <v>10</v>
+      </c>
+      <c r="I257" s="1">
+        <v>44697</v>
+      </c>
+      <c r="J257">
+        <f t="shared" si="17"/>
+        <v>60.6</v>
+      </c>
+      <c r="K257" t="s">
+        <v>118</v>
+      </c>
+      <c r="L257" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="258" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A258">
+        <v>13</v>
+      </c>
+      <c r="B258" t="s">
+        <v>12</v>
+      </c>
+      <c r="C258" t="s">
+        <v>161</v>
+      </c>
+      <c r="D258" t="s">
+        <v>97</v>
+      </c>
+      <c r="E258">
+        <v>17</v>
+      </c>
+      <c r="F258">
+        <v>198</v>
+      </c>
+      <c r="G258">
+        <v>191.9</v>
+      </c>
+      <c r="H258">
+        <f t="shared" si="16"/>
+        <v>6.0999999999999943</v>
+      </c>
+      <c r="I258" s="1">
+        <v>44697</v>
+      </c>
+      <c r="J258">
+        <f t="shared" si="17"/>
+        <v>60.6</v>
+      </c>
+      <c r="K258" t="s">
+        <v>118</v>
+      </c>
+      <c r="L258" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="259" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A259">
+        <v>13</v>
+      </c>
+      <c r="B259" t="s">
+        <v>12</v>
+      </c>
+      <c r="C259" t="s">
+        <v>199</v>
+      </c>
+      <c r="D259" t="s">
+        <v>46</v>
+      </c>
+      <c r="E259">
+        <v>18</v>
+      </c>
+      <c r="F259">
+        <v>211</v>
+      </c>
+      <c r="G259">
+        <v>211</v>
+      </c>
+      <c r="H259">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="I259" s="1">
+        <v>44697</v>
+      </c>
+      <c r="J259">
+        <f t="shared" si="17"/>
+        <v>60.6</v>
+      </c>
+      <c r="K259" t="s">
+        <v>118</v>
+      </c>
+      <c r="L259" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="260" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A260">
+        <v>13</v>
+      </c>
+      <c r="B260" t="s">
+        <v>26</v>
+      </c>
+      <c r="C260" t="s">
+        <v>188</v>
+      </c>
+      <c r="D260" t="s">
+        <v>70</v>
+      </c>
+      <c r="E260">
+        <v>19</v>
+      </c>
+      <c r="F260">
+        <v>222</v>
+      </c>
+      <c r="G260">
+        <v>222</v>
+      </c>
+      <c r="H260">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="I260" s="1">
+        <v>44697</v>
+      </c>
+      <c r="J260">
+        <f t="shared" si="17"/>
+        <v>60.6</v>
+      </c>
+      <c r="K260" t="s">
+        <v>118</v>
+      </c>
+      <c r="L260" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="261" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A261">
+        <v>13</v>
+      </c>
+      <c r="B261" t="s">
+        <v>12</v>
+      </c>
+      <c r="C261" t="s">
+        <v>101</v>
+      </c>
+      <c r="D261" t="s">
+        <v>100</v>
+      </c>
+      <c r="E261">
+        <v>20</v>
+      </c>
+      <c r="F261">
+        <v>235</v>
+      </c>
+      <c r="G261">
+        <v>235</v>
+      </c>
+      <c r="H261">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="I261" s="1">
+        <v>44697</v>
+      </c>
+      <c r="J261">
+        <f t="shared" si="17"/>
+        <v>60.6</v>
+      </c>
+      <c r="K261" t="s">
+        <v>118</v>
+      </c>
+      <c r="L261" t="s">
+        <v>127</v>
       </c>
     </row>
   </sheetData>

</xml_diff>